<commit_message>
Updated Test Data. Signed-off-by: Admin <Admin@CTNL0060.crestechad.com>
</commit_message>
<xml_diff>
--- a/ExecutionTestData/Batch1/TestData.xlsx
+++ b/ExecutionTestData/Batch1/TestData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Capabilities" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="147">
   <si>
     <t>ApplicationActivity</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>DBS</t>
+  </si>
+  <si>
+    <t>sakshi.juneja@crestechsoftware.com</t>
+  </si>
+  <si>
+    <t>t68k6kw68ywjv2y9zwfr9r3t</t>
   </si>
   <si>
     <t>S2021219EUID</t>
@@ -273,6 +279,9 @@
   </si>
   <si>
     <t>XIAOMI_RedmiNote7Pro_Android_9.0.0_059d9</t>
+  </si>
+  <si>
+    <t>8.1.0</t>
   </si>
   <si>
     <t>9.0.0</t>
@@ -604,15 +613,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -921,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,13 +1043,13 @@
         <v>5</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>22</v>
@@ -1084,13 +1093,13 @@
         <v>5</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>22</v>
@@ -1104,41 +1113,122 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="12" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="P1" s="18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1148,19 +1238,97 @@
       <c r="C3" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K4" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1170,8 +1338,47 @@
       <c r="C5" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1181,8 +1388,47 @@
       <c r="C6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="O6" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1192,8 +1438,47 @@
       <c r="C7" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1203,8 +1488,47 @@
       <c r="C8" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1214,8 +1538,47 @@
       <c r="C9" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="11">
+        <v>3</v>
+      </c>
+      <c r="E9" s="11">
+        <v>4</v>
+      </c>
+      <c r="F9" s="11">
+        <v>5</v>
+      </c>
+      <c r="G9" s="11">
+        <v>6</v>
+      </c>
+      <c r="H9" s="11">
+        <v>7</v>
+      </c>
+      <c r="I9" s="11">
+        <v>8</v>
+      </c>
+      <c r="J9" s="11">
+        <v>9</v>
+      </c>
+      <c r="K9" s="11">
+        <v>10</v>
+      </c>
+      <c r="L9" s="11">
+        <v>11</v>
+      </c>
+      <c r="M9" s="11">
+        <v>12</v>
+      </c>
+      <c r="N9" s="11">
+        <v>13</v>
+      </c>
+      <c r="O9" s="11">
+        <v>14</v>
+      </c>
+      <c r="P9" s="11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1225,12 +1588,52 @@
       <c r="C10" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
-    </row>
-    <row r="13" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="D12" s="12"/>
+    </row>
+    <row r="13" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="45" orientation="portrait" r:id="rId1"/>
@@ -1332,72 +1735,72 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O2" t="s">
+        <v>53</v>
+      </c>
+      <c r="P2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>55</v>
+      </c>
+      <c r="R2" t="s">
+        <v>56</v>
+      </c>
+      <c r="S2" t="s">
+        <v>57</v>
+      </c>
+      <c r="T2" t="s">
         <v>58</v>
       </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L2" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" t="s">
-        <v>49</v>
-      </c>
-      <c r="N2" t="s">
-        <v>50</v>
-      </c>
-      <c r="O2" t="s">
-        <v>51</v>
-      </c>
-      <c r="P2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>53</v>
-      </c>
-      <c r="R2" t="s">
-        <v>54</v>
-      </c>
-      <c r="S2" t="s">
-        <v>55</v>
-      </c>
-      <c r="T2" t="s">
-        <v>56</v>
-      </c>
       <c r="U2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
+      <c r="A3" s="15"/>
       <c r="B3">
         <v>121212</v>
       </c>
@@ -1461,32 +1864,32 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -1513,33 +1916,33 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
-        <v>65</v>
+      <c r="A12" s="16" t="s">
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F12" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H12" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="16"/>
       <c r="B13">
         <v>121212</v>
       </c>
@@ -1564,32 +1967,32 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1616,328 +2019,328 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="18" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="16" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="16" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="16" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="16" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="16" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="16" t="s">
-        <v>77</v>
-      </c>
-    </row>
     <row r="37" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="16" t="s">
-        <v>114</v>
+      <c r="A37" s="18" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="16" t="s">
-        <v>115</v>
+      <c r="A38" s="18" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="16" t="s">
-        <v>116</v>
+      <c r="A39" s="18" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="16" t="s">
-        <v>117</v>
+      <c r="A40" s="18" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="16" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="16" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="16" t="s">
-        <v>120</v>
+      <c r="A41" s="18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="18" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="16" t="s">
-        <v>121</v>
+      <c r="A44" s="18" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="16" t="s">
-        <v>122</v>
+      <c r="A45" s="18" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="16" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="16" t="s">
-        <v>124</v>
+      <c r="A46" s="18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="18" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="16" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="16" t="s">
-        <v>126</v>
+      <c r="A48" s="18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="18" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="16" t="s">
-        <v>127</v>
+      <c r="A50" s="18" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="16" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="16" t="s">
-        <v>129</v>
+      <c r="A51" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="18" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="16" t="s">
-        <v>130</v>
+      <c r="A53" s="18" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="16" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="16" t="s">
-        <v>133</v>
+      <c r="A54" s="18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="18" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="16" t="s">
-        <v>134</v>
+      <c r="A57" s="18" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="16" t="s">
-        <v>135</v>
+      <c r="A58" s="18" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="16" t="s">
-        <v>136</v>
+      <c r="A59" s="18" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="16" t="s">
-        <v>137</v>
+      <c r="A60" s="18" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="16" t="s">
-        <v>138</v>
+      <c r="A61" s="18" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="16" t="s">
-        <v>139</v>
+      <c r="A62" s="18" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="16" t="s">
-        <v>140</v>
+      <c r="A63" s="18" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="16" t="s">
-        <v>141</v>
+      <c r="A64" s="18" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="16" t="s">
-        <v>142</v>
+      <c r="A65" s="18" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TestData Added. Signed-off-by: Admin <Admin@CTNL0060.crestechad.com>
</commit_message>
<xml_diff>
--- a/ExecutionTestData/Batch1/TestData.xlsx
+++ b/ExecutionTestData/Batch1/TestData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="148">
   <si>
     <t>ApplicationActivity</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>webkitDebugProxyPort</t>
-  </si>
-  <si>
-    <t>app</t>
   </si>
   <si>
     <t>Device</t>
@@ -480,6 +477,12 @@
   </si>
   <si>
     <t>11.0.0</t>
+  </si>
+  <si>
+    <t>EndPoint</t>
+  </si>
+  <si>
+    <t>https://device.pcloudy.com</t>
   </si>
 </sst>
 </file>
@@ -613,15 +616,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -930,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,7 +969,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>19</v>
+        <v>146</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -1010,13 +1013,13 @@
         <v>8</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>27</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>5</v>
+        <v>147</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>5</v>
@@ -1043,16 +1046,16 @@
         <v>5</v>
       </c>
       <c r="M2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="N2" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="O2" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1063,10 +1066,10 @@
         <v>5</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>5</v>
+        <v>26</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>147</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>15</v>
@@ -1078,7 +1081,7 @@
         <v>5</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>5</v>
@@ -1093,16 +1096,16 @@
         <v>5</v>
       </c>
       <c r="M3" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="N3" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="O3" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1116,7 +1119,7 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,107 +1133,107 @@
   <sheetData>
     <row r="1" spans="1:16" s="12" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="F1" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="G1" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="H1" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="I1" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="J1" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="K1" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="L1" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="M1" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="N1" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="O1" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="P1" s="16" t="s">
         <v>95</v>
-      </c>
-      <c r="P1" s="18" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="L2" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>8</v>
@@ -1280,257 +1283,257 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="K4" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="L4" s="17" t="s">
+      <c r="M4" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="M4" s="17" t="s">
+      <c r="N4" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="N4" s="17" t="s">
+      <c r="O4" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="O4" s="17" t="s">
+      <c r="P4" s="15" t="s">
         <v>53</v>
-      </c>
-      <c r="P4" s="17" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="L6" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="M6" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="N6" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="O6" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="P6" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6" s="15" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="11">
         <v>1</v>
@@ -1580,52 +1583,52 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1735,72 +1738,72 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>60</v>
+      <c r="A2" s="17" t="s">
+        <v>59</v>
       </c>
       <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" t="s">
         <v>49</v>
       </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>50</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>51</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>52</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>53</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>54</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>55</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>56</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>57</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>58</v>
       </c>
-      <c r="U2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
+      <c r="A3" s="17"/>
       <c r="B3">
         <v>121212</v>
       </c>
@@ -1864,32 +1867,32 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -1916,33 +1919,33 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" t="s">
         <v>67</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>68</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>69</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>70</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>71</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>72</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>73</v>
       </c>
-      <c r="H12" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
+      <c r="A13" s="18"/>
       <c r="B13">
         <v>121212</v>
       </c>
@@ -1967,32 +1970,32 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2019,328 +2022,328 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+    <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+    <row r="4" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+    <row r="5" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+    <row r="6" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+    <row r="7" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+    <row r="8" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+    <row r="9" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+    <row r="10" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
+    <row r="11" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+    <row r="12" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
+    <row r="13" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
+    <row r="14" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
+    <row r="15" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
+    <row r="16" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
+    <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="18" t="s">
+    <row r="18" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
+    <row r="19" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="16" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
+    <row r="20" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18" t="s">
+    <row r="21" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="16" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="18" t="s">
+    <row r="22" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="16" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="18" t="s">
+    <row r="23" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="16" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="18" t="s">
+    <row r="24" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="16" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="18" t="s">
+    <row r="25" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="16" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="18" t="s">
+    <row r="26" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="16" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="18" t="s">
+    <row r="27" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="16" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="18" t="s">
+    <row r="28" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="16" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="18" t="s">
+    <row r="29" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="16" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="18" t="s">
+    <row r="30" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="16" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="18" t="s">
+    <row r="31" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="16" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="18" t="s">
+    <row r="32" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="16" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="18" t="s">
+    <row r="33" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="16" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="18" t="s">
+    <row r="34" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="16" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="18" t="s">
+    <row r="35" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="18" t="s">
+    <row r="36" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="16" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="18" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="18" t="s">
+    <row r="38" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="16" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="18" t="s">
+    <row r="39" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="16" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="18" t="s">
+    <row r="40" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="18" t="s">
+    <row r="41" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="16" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="18" t="s">
+    <row r="42" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="16" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="18" t="s">
+    <row r="43" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="16" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="18" t="s">
+    <row r="44" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="16" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="18" t="s">
+    <row r="45" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="16" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="18" t="s">
+    <row r="46" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="16" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="18" t="s">
+    <row r="47" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="16" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="18" t="s">
+    <row r="48" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="16" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="18" t="s">
+    <row r="49" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="16" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="18" t="s">
+    <row r="50" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="16" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="18" t="s">
+    <row r="51" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="16" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="18" t="s">
+    <row r="52" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="16" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="18" t="s">
+    <row r="53" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="16" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="18" t="s">
+    <row r="54" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="16" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="18" t="s">
+    <row r="55" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="18" t="s">
+    <row r="56" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="16" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="18" t="s">
+    <row r="57" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="16" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="18" t="s">
+    <row r="58" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="16" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="18" t="s">
+    <row r="59" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="16" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="18" t="s">
+    <row r="60" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="16" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="18" t="s">
+    <row r="61" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="16" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="18" t="s">
+    <row r="62" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="16" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="18" t="s">
+    <row r="63" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="18" t="s">
+    <row r="64" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="16" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="18" t="s">
+    <row r="65" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="16" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="18" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test Data Updation. Signed-off-by: Admin <Admin@CTNL0060.crestechad.com>
</commit_message>
<xml_diff>
--- a/ExecutionTestData/Batch1/TestData.xlsx
+++ b/ExecutionTestData/Batch1/TestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="150">
   <si>
     <t>ApplicationActivity</t>
   </si>
@@ -278,12 +278,6 @@
     <t>XIAOMI_RedmiNote7Pro_Android_9.0.0_059d9</t>
   </si>
   <si>
-    <t>8.1.0</t>
-  </si>
-  <si>
-    <t>9.0.0</t>
-  </si>
-  <si>
     <t>GOOGLE_Pixel5_Android_11.0.0_21d59</t>
   </si>
   <si>
@@ -483,13 +477,25 @@
   </si>
   <si>
     <t>https://device.pcloudy.com</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyNote20_Android_11.0.0_765c8</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyNote20_Android_12.0.0_2b7fa</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyS10_Android_12.0.0_d2537</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -531,8 +537,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -545,8 +557,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF00FFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFEA9999"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -569,14 +611,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -595,17 +666,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -620,12 +685,33 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -933,178 +1019,178 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="48.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="37" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="63.5703125" style="4" customWidth="1"/>
-    <col min="16" max="16" width="26.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="14.7109375" style="4"/>
+    <col min="1" max="1" width="22.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="48.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="37" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="63.5703125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="26.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="14.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="O2" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1116,10 +1202,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:X13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,160 +1215,219 @@
     <col min="4" max="4" width="35.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="41" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="44.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="12" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" s="16" t="s">
+      <c r="B1" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="C1" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="N1" s="16" t="s">
+      <c r="D1" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="O1" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E1" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="O1" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="P1" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q1" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="R1" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="S1" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="T1" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="U1" s="30" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="S2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="T2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="U2" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="P3" s="17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="Q3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="R3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="S3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="U3" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="15" t="s">
@@ -1330,74 +1475,110 @@
       <c r="P4" s="15" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="Q4" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="R4" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="S4" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="T4" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="U4" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="16" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="Q5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="R5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="S5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="T5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="15" t="s">
         <v>33</v>
       </c>
       <c r="G6" s="15" t="s">
@@ -1430,213 +1611,288 @@
       <c r="P6" s="15" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="Q6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="R6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="S6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="T6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="U6" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" s="16" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="Q7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="R7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="S7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="T7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="U7" s="16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L8" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="M8" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N8" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="P8" s="16" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="Q8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="R8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="S8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="T8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="U8" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="18">
         <v>1</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="18">
         <v>2</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="18">
         <v>3</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="18">
         <v>4</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="18">
         <v>5</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="18">
         <v>6</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="18">
         <v>7</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="18">
         <v>8</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="18">
         <v>9</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="18">
         <v>10</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="18">
         <v>11</v>
       </c>
-      <c r="M9" s="11">
+      <c r="M9" s="18">
         <v>12</v>
       </c>
-      <c r="N9" s="11">
+      <c r="N9" s="18">
         <v>13</v>
       </c>
-      <c r="O9" s="11">
+      <c r="O9" s="18">
         <v>14</v>
       </c>
-      <c r="P9" s="11">
+      <c r="P9" s="18">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="Q9" s="18">
+        <v>16</v>
+      </c>
+      <c r="R9" s="18">
+        <v>17</v>
+      </c>
+      <c r="S9" s="18">
+        <v>18</v>
+      </c>
+      <c r="T9" s="18">
+        <v>19</v>
+      </c>
+      <c r="U9" s="18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="M10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="N10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="O10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="P10" s="16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-    </row>
-    <row r="13" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="Q10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="R10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="S10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="T10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="U10" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="45" orientation="portrait" r:id="rId1"/>
@@ -1647,8 +1903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:P3"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1738,7 +1994,7 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>59</v>
       </c>
       <c r="B2" t="s">
@@ -1803,7 +2059,7 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
+      <c r="A3" s="19"/>
       <c r="B3">
         <v>121212</v>
       </c>
@@ -1866,32 +2122,32 @@
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="10" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="9" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="9" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1919,7 +2175,7 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="20" t="s">
         <v>66</v>
       </c>
       <c r="B12" t="s">
@@ -1945,7 +2201,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="20"/>
       <c r="B13">
         <v>121212</v>
       </c>
@@ -1969,32 +2225,32 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="10" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="9" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="9" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="9" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="9" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2022,328 +2278,328 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+    <row r="4" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+    <row r="5" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+    <row r="6" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+    <row r="7" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+    <row r="8" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+    <row r="9" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+    <row r="10" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+    <row r="11" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
+    <row r="12" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+    <row r="13" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
+    <row r="14" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
+    <row r="15" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
+    <row r="16" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
+    <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
+    <row r="18" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
+    <row r="19" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="13" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
+    <row r="20" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
+    <row r="21" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="13" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
+    <row r="22" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="13" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="16" t="s">
+    <row r="23" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="13" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
+    <row r="24" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="13" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
+    <row r="25" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="13" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="16" t="s">
+    <row r="26" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="13" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="16" t="s">
+    <row r="27" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="13" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="16" t="s">
+    <row r="28" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="13" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
+    <row r="29" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="13" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="16" t="s">
+    <row r="30" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="13" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="16" t="s">
+    <row r="31" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="13" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="16" t="s">
+    <row r="32" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="13" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="16" t="s">
+    <row r="33" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="13" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="16" t="s">
+    <row r="34" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="13" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="16" t="s">
+    <row r="35" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="13" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="16" t="s">
+    <row r="36" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="13" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="16" t="s">
+    <row r="38" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="13" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="16" t="s">
+    <row r="39" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="13" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="16" t="s">
+    <row r="40" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="13" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="16" t="s">
+    <row r="41" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="13" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="16" t="s">
+    <row r="42" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="13" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="16" t="s">
+    <row r="43" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="13" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="16" t="s">
+    <row r="44" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="13" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="16" t="s">
+    <row r="45" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="13" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="16" t="s">
+    <row r="46" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="13" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="16" t="s">
+    <row r="47" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="13" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="16" t="s">
+    <row r="48" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="13" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="16" t="s">
+    <row r="49" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="16" t="s">
+    <row r="50" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="13" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="16" t="s">
+    <row r="51" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="13" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="16" t="s">
+    <row r="52" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="13" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="16" t="s">
+    <row r="53" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="13" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="16" t="s">
+    <row r="54" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="13" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="16" t="s">
+    <row r="55" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="13" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="16" t="s">
+    <row r="56" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="13" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="16" t="s">
+    <row r="57" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="13" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="16" t="s">
+    <row r="58" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="13" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="16" t="s">
+    <row r="59" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="13" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="16" t="s">
+    <row r="60" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="13" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="16" t="s">
+    <row r="61" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="13" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="16" t="s">
+    <row r="62" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="13" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="16" t="s">
+    <row r="63" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="13" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="16" t="s">
+    <row r="64" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="13" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="16" t="s">
+    <row r="65" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="13" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="16" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="16" t="s">
-        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Handle Digibank Alert on Samsung Devices. Signed-off-by: Admin <Admin@CTNL0060.crestechad.com>
</commit_message>
<xml_diff>
--- a/ExecutionTestData/Batch1/TestData.xlsx
+++ b/ExecutionTestData/Batch1/TestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="150">
   <si>
     <t>ApplicationActivity</t>
   </si>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>Xiaomi</t>
-  </si>
-  <si>
-    <t>121212</t>
   </si>
   <si>
     <t>AppName</t>
@@ -479,23 +476,26 @@
     <t>https://device.pcloudy.com</t>
   </si>
   <si>
-    <t>SAMSUNG_GalaxyNote20_Android_11.0.0_765c8</t>
-  </si>
-  <si>
-    <t>SAMSUNG_GalaxyNote20_Android_12.0.0_2b7fa</t>
-  </si>
-  <si>
-    <t>SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t>SAMSUNG_GalaxyS10_Android_12.0.0_d2537</t>
+    <t>iWEALTH</t>
+  </si>
+  <si>
+    <t>NSTRAX15</t>
+  </si>
+  <si>
+    <t>425455</t>
+  </si>
+  <si>
+    <t>NSTRAX10</t>
+  </si>
+  <si>
+    <t>872465</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -537,14 +537,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -566,25 +560,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor rgb="FF00FFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FFEA9999"/>
       </patternFill>
     </fill>
   </fills>
@@ -646,7 +622,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -696,22 +672,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1055,7 +1023,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1105,7 +1073,7 @@
         <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>5</v>
@@ -1132,13 +1100,13 @@
         <v>5</v>
       </c>
       <c r="M2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="O2" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>21</v>
@@ -1155,7 +1123,7 @@
         <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>15</v>
@@ -1182,13 +1150,13 @@
         <v>5</v>
       </c>
       <c r="M3" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="O3" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>21</v>
@@ -1202,166 +1170,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="41" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="42.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="42.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="I1" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="J1" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="K1" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="L1" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="O1" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="P1" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q1" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="R1" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="S1" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="T1" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="U1" s="30" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="M2" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="O2" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q2" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="R2" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="S2" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="T2" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="U2" s="16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>22</v>
       </c>
@@ -1371,198 +1213,36 @@
       <c r="C3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="O3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="P3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="R3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="S3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="T3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="U3" s="17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>48</v>
+        <v>148</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="M4" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="N4" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="O4" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="P4" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q4" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="R4" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="S4" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="T4" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="U4" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>34</v>
+        <v>149</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="N5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="O5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="P5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="R5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="S5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="T5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="U5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="V5" s="12"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>27</v>
       </c>
@@ -1572,62 +1252,8 @@
       <c r="C6" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="M6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="N6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="O6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="P6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="R6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="S6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="T6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="U6" s="15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>28</v>
       </c>
@@ -1637,62 +1263,8 @@
       <c r="C7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="K7" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="M7" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="N7" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="O7" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="P7" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q7" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="R7" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="S7" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="T7" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="U7" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>29</v>
       </c>
@@ -1702,62 +1274,8 @@
       <c r="C8" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="N8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="O8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="P8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="R8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="S8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="T8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="U8" s="16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>31</v>
       </c>
@@ -1767,132 +1285,23 @@
       <c r="C9" s="18">
         <v>2</v>
       </c>
-      <c r="D9" s="18">
-        <v>3</v>
-      </c>
-      <c r="E9" s="18">
-        <v>4</v>
-      </c>
-      <c r="F9" s="18">
-        <v>5</v>
-      </c>
-      <c r="G9" s="18">
-        <v>6</v>
-      </c>
-      <c r="H9" s="18">
-        <v>7</v>
-      </c>
-      <c r="I9" s="18">
-        <v>8</v>
-      </c>
-      <c r="J9" s="18">
-        <v>9</v>
-      </c>
-      <c r="K9" s="18">
-        <v>10</v>
-      </c>
-      <c r="L9" s="18">
-        <v>11</v>
-      </c>
-      <c r="M9" s="18">
-        <v>12</v>
-      </c>
-      <c r="N9" s="18">
-        <v>13</v>
-      </c>
-      <c r="O9" s="18">
-        <v>14</v>
-      </c>
-      <c r="P9" s="18">
-        <v>15</v>
-      </c>
-      <c r="Q9" s="18">
-        <v>16</v>
-      </c>
-      <c r="R9" s="18">
-        <v>17</v>
-      </c>
-      <c r="S9" s="18">
-        <v>18</v>
-      </c>
-      <c r="T9" s="18">
-        <v>19</v>
-      </c>
-      <c r="U9" s="18">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>36</v>
-      </c>
       <c r="C10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="K10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="L10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="M10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="N10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="O10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="P10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="R10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="S10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="T10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="U10" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-    </row>
-    <row r="13" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="13" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="45" orientation="portrait" r:id="rId1"/>
@@ -1994,72 +1403,72 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>59</v>
+      <c r="A2" s="21" t="s">
+        <v>58</v>
       </c>
       <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" t="s">
         <v>48</v>
       </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>49</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>50</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>51</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>52</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>53</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>54</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>55</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>56</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>57</v>
       </c>
-      <c r="U2" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
+      <c r="A3" s="21"/>
       <c r="B3">
         <v>121212</v>
       </c>
@@ -2123,32 +1532,32 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -2175,33 +1584,33 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" t="s">
         <v>66</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>67</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>68</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>69</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>70</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>71</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>72</v>
       </c>
-      <c r="H12" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+      <c r="A13" s="22"/>
       <c r="B13">
         <v>121212</v>
       </c>
@@ -2226,32 +1635,32 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2279,327 +1688,327 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code Modification Signed-off-by: Admin <Admin@CTNL0060.crestechad.com>
</commit_message>
<xml_diff>
--- a/ExecutionTestData/Batch1/TestData.xlsx
+++ b/ExecutionTestData/Batch1/TestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="150">
   <si>
     <t>ApplicationActivity</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Xiaomi</t>
+  </si>
+  <si>
+    <t>121212</t>
   </si>
   <si>
     <t>AppName</t>
@@ -476,26 +479,23 @@
     <t>https://device.pcloudy.com</t>
   </si>
   <si>
-    <t>iWEALTH</t>
-  </si>
-  <si>
-    <t>NSTRAX15</t>
-  </si>
-  <si>
-    <t>425455</t>
-  </si>
-  <si>
-    <t>NSTRAX10</t>
-  </si>
-  <si>
-    <t>872465</t>
+    <t>SAMSUNG_GalaxyNote20_Android_11.0.0_765c8</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyNote20_Android_12.0.0_2b7fa</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyS10_Android_12.0.0_d2537</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -537,8 +537,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -560,7 +566,25 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor rgb="FF00FFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFEA9999"/>
       </patternFill>
     </fill>
   </fills>
@@ -622,7 +646,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -672,14 +696,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1023,7 +1055,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1073,7 +1105,7 @@
         <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>5</v>
@@ -1100,13 +1132,13 @@
         <v>5</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>21</v>
@@ -1123,7 +1155,7 @@
         <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>15</v>
@@ -1150,13 +1182,13 @@
         <v>5</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>21</v>
@@ -1170,40 +1202,166 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:X13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="41" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="44.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="C1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C1" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="O1" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="P1" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q1" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="R1" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="S1" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="T1" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="U1" s="30" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="S2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="T2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="U2" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>22</v>
       </c>
@@ -1213,36 +1371,198 @@
       <c r="C3" s="17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="O3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="R3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="S3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="U3" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>148</v>
+        <v>48</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="P4" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q4" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="R4" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="S4" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="T4" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="U4" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>149</v>
+        <v>34</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="R5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="S5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="T5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>27</v>
       </c>
@@ -1252,8 +1572,62 @@
       <c r="C6" s="15" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="R6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="S6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="T6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="U6" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>28</v>
       </c>
@@ -1263,8 +1637,62 @@
       <c r="C7" s="16" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="R7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="S7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="T7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="U7" s="16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>29</v>
       </c>
@@ -1274,8 +1702,62 @@
       <c r="C8" s="16" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="R8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="S8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="T8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="U8" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>31</v>
       </c>
@@ -1285,23 +1767,132 @@
       <c r="C9" s="18">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="18">
+        <v>3</v>
+      </c>
+      <c r="E9" s="18">
+        <v>4</v>
+      </c>
+      <c r="F9" s="18">
+        <v>5</v>
+      </c>
+      <c r="G9" s="18">
+        <v>6</v>
+      </c>
+      <c r="H9" s="18">
+        <v>7</v>
+      </c>
+      <c r="I9" s="18">
+        <v>8</v>
+      </c>
+      <c r="J9" s="18">
+        <v>9</v>
+      </c>
+      <c r="K9" s="18">
+        <v>10</v>
+      </c>
+      <c r="L9" s="18">
+        <v>11</v>
+      </c>
+      <c r="M9" s="18">
+        <v>12</v>
+      </c>
+      <c r="N9" s="18">
+        <v>13</v>
+      </c>
+      <c r="O9" s="18">
+        <v>14</v>
+      </c>
+      <c r="P9" s="18">
+        <v>15</v>
+      </c>
+      <c r="Q9" s="18">
+        <v>16</v>
+      </c>
+      <c r="R9" s="18">
+        <v>17</v>
+      </c>
+      <c r="S9" s="18">
+        <v>18</v>
+      </c>
+      <c r="T9" s="18">
+        <v>19</v>
+      </c>
+      <c r="U9" s="18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="L10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="N10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="O10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="P10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="R10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="S10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="T10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="U10" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
-    </row>
-    <row r="13" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="45" orientation="portrait" r:id="rId1"/>
@@ -1403,72 +1994,72 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>54</v>
+      </c>
+      <c r="R2" t="s">
+        <v>55</v>
+      </c>
+      <c r="S2" t="s">
+        <v>56</v>
+      </c>
+      <c r="T2" t="s">
+        <v>57</v>
+      </c>
+      <c r="U2" t="s">
         <v>58</v>
       </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L2" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" t="s">
-        <v>49</v>
-      </c>
-      <c r="N2" t="s">
-        <v>50</v>
-      </c>
-      <c r="O2" t="s">
-        <v>51</v>
-      </c>
-      <c r="P2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>53</v>
-      </c>
-      <c r="R2" t="s">
-        <v>54</v>
-      </c>
-      <c r="S2" t="s">
-        <v>55</v>
-      </c>
-      <c r="T2" t="s">
-        <v>56</v>
-      </c>
-      <c r="U2" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
+      <c r="A3" s="19"/>
       <c r="B3">
         <v>121212</v>
       </c>
@@ -1532,32 +2123,32 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -1584,33 +2175,33 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
-        <v>65</v>
+      <c r="A12" s="20" t="s">
+        <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
+      <c r="A13" s="20"/>
       <c r="B13">
         <v>121212</v>
       </c>
@@ -1635,32 +2226,32 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1688,327 +2279,327 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="13" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="13" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="13" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="13" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="13" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="13" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>